<commit_message>
Fix get categories issue
</commit_message>
<xml_diff>
--- a/backend/src/transactions/categories.xlsx
+++ b/backend/src/transactions/categories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harel\Elazar Harel\taxmyself\taxmyself-dev\backend\src\transactions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5855E3B-C159-47FE-B9A1-30CC18E43636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4709F3BC-7A76-429F-A507-B3CAB4BBB06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="categories" sheetId="1" r:id="rId1"/>
@@ -138,12 +138,6 @@
     <t>categoryId</t>
   </si>
   <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>subCategory</t>
-  </si>
-  <si>
     <t>taxPercent</t>
   </si>
   <si>
@@ -160,6 +154,12 @@
   </si>
   <si>
     <t>מלאי</t>
+  </si>
+  <si>
+    <t>categoryName</t>
+  </si>
+  <si>
+    <t>subCategoryName</t>
   </si>
 </sst>
 </file>
@@ -493,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -511,28 +511,28 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -1374,7 +1374,7 @@
         <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C34">
         <v>6</v>

</xml_diff>

<commit_message>
Disable duplicate categories loading
</commit_message>
<xml_diff>
--- a/backend/src/transactions/categories.xlsx
+++ b/backend/src/transactions/categories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harel\Elazar Harel\taxmyself\taxmyself-dev\backend\src\transactions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304A79C0-51F3-457A-8D61-8C497BE9F479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC8271E-2DE2-473B-A226-23636CCC18BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="categories" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="47">
   <si>
     <t>דלק</t>
   </si>
@@ -157,6 +157,15 @@
   </si>
   <si>
     <t>subCategoryName</t>
+  </si>
+  <si>
+    <t>דוח שנתי</t>
+  </si>
+  <si>
+    <t>תרומה מוכרת</t>
+  </si>
+  <si>
+    <t>ביטוח חיים</t>
   </si>
 </sst>
 </file>
@@ -488,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1289,6 +1298,52 @@
         <v>1</v>
       </c>
     </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add isExpense field to the categories entity
</commit_message>
<xml_diff>
--- a/backend/src/transactions/categories.xlsx
+++ b/backend/src/transactions/categories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harel\Elazar Harel\taxmyself\taxmyself-dev\backend\src\transactions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC8271E-2DE2-473B-A226-23636CCC18BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203BDE8D-01BD-4988-A6D1-BB2303B2EDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="categories" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
   <si>
     <t>דלק</t>
   </si>
@@ -166,6 +166,27 @@
   </si>
   <si>
     <t>ביטוח חיים</t>
+  </si>
+  <si>
+    <t>isExpense</t>
+  </si>
+  <si>
+    <t>הכנסה מעסק</t>
+  </si>
+  <si>
+    <t>משכורת</t>
+  </si>
+  <si>
+    <t>ביטוח לאומי</t>
+  </si>
+  <si>
+    <t>מילואים</t>
+  </si>
+  <si>
+    <t>קצבת ילדים</t>
+  </si>
+  <si>
+    <t>דמי לידה</t>
   </si>
 </sst>
 </file>
@@ -497,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -511,7 +532,8 @@
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="18.296875" customWidth="1"/>
     <col min="6" max="6" width="16.296875" customWidth="1"/>
-    <col min="7" max="7" width="22.59765625" customWidth="1"/>
+    <col min="7" max="7" width="27.796875" customWidth="1"/>
+    <col min="8" max="8" width="21.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -536,7 +558,9 @@
       <c r="G1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -561,6 +585,9 @@
       <c r="G2">
         <v>1</v>
       </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -584,6 +611,9 @@
       <c r="G3">
         <v>1</v>
       </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -607,6 +637,9 @@
       <c r="G4">
         <v>1</v>
       </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -630,6 +663,9 @@
       <c r="G5">
         <v>1</v>
       </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -653,6 +689,9 @@
       <c r="G6">
         <v>1</v>
       </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -676,6 +715,9 @@
       <c r="G7">
         <v>1</v>
       </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -699,6 +741,9 @@
       <c r="G8">
         <v>1</v>
       </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -722,6 +767,9 @@
       <c r="G9">
         <v>1</v>
       </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -745,6 +793,9 @@
       <c r="G10">
         <v>1</v>
       </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -768,6 +819,9 @@
       <c r="G11">
         <v>1</v>
       </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -791,6 +845,9 @@
       <c r="G12">
         <v>1</v>
       </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -814,6 +871,9 @@
       <c r="G13">
         <v>1</v>
       </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -837,6 +897,9 @@
       <c r="G14">
         <v>1</v>
       </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -860,6 +923,9 @@
       <c r="G15">
         <v>1</v>
       </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -883,8 +949,11 @@
       <c r="G16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -906,8 +975,11 @@
       <c r="G17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -929,8 +1001,11 @@
       <c r="G18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -952,8 +1027,11 @@
       <c r="G19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -975,8 +1053,11 @@
       <c r="G20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -998,8 +1079,11 @@
       <c r="G21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1021,8 +1105,11 @@
       <c r="G22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1044,8 +1131,11 @@
       <c r="G23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1067,8 +1157,11 @@
       <c r="G24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1090,8 +1183,11 @@
       <c r="G25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1113,8 +1209,11 @@
       <c r="G26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1136,8 +1235,11 @@
       <c r="G27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1159,8 +1261,11 @@
       <c r="G28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1182,8 +1287,11 @@
       <c r="G29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1205,8 +1313,11 @@
       <c r="G30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1228,8 +1339,11 @@
       <c r="G31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1251,8 +1365,11 @@
       <c r="G32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1274,8 +1391,11 @@
       <c r="G33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1297,8 +1417,11 @@
       <c r="G34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -1320,8 +1443,11 @@
       <c r="G35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -1341,6 +1467,139 @@
         <v>0</v>
       </c>
       <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
         <v>0</v>
       </c>
     </row>

</xml_diff>